<commit_message>
PROS-5749 - CCRU merging PROD to SAND
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/Convenience Spirits 2018.xlsx
+++ b/Projects/CCRU_SAND/Data/Convenience Spirits 2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="81">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -410,30 +410,30 @@
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.45"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="35.1336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="30.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.0647773279352"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="19" min="15" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="40.0607287449393"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="40.3846153846154"/>
     <col collapsed="false" hidden="false" max="28" min="24" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="8.57085020242915"/>
@@ -807,7 +807,9 @@
       <c r="G6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K6" s="0"/>
+      <c r="K6" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="L6" s="1" t="s">
         <v>45</v>
       </c>
@@ -982,6 +984,9 @@
       <c r="G9" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="K9" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="L9" s="1" t="s">
         <v>45</v>
       </c>
@@ -1040,6 +1045,9 @@
       </c>
       <c r="J10" s="0" t="s">
         <v>77</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>45</v>

</xml_diff>